<commit_message>
edit import samples & add pagination
</commit_message>
<xml_diff>
--- a/import_grade_sample.xlsx
+++ b/import_grade_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\新笔记本 2017.2.11起\工程项目\清华大学电子工程系奖学金申报系统\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\新笔记本 2017.2.11起\工程项目\清华大学电子工程系奖学金申报系统\代码\前端\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -352,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -369,13 +365,13 @@
         <v>2013011001</v>
       </c>
       <c r="B1">
-        <v>3.4</v>
+        <v>3.99</v>
       </c>
       <c r="C1">
         <v>1</v>
       </c>
       <c r="D1">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -383,13 +379,13 @@
         <v>2013011002</v>
       </c>
       <c r="B2">
-        <v>3.3</v>
+        <v>3.98</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -397,13 +393,13 @@
         <v>2013011003</v>
       </c>
       <c r="B3">
-        <v>3.2</v>
+        <v>3.97</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -411,13 +407,363 @@
         <v>2013011004</v>
       </c>
       <c r="B4">
-        <v>3.1</v>
+        <v>3.96</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2013011005</v>
+      </c>
+      <c r="B5">
+        <v>3.95</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2013011006</v>
+      </c>
+      <c r="B6">
+        <v>3.94</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>2013011007</v>
+      </c>
+      <c r="B7">
+        <v>3.93</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>2013011008</v>
+      </c>
+      <c r="B8">
+        <v>3.92</v>
+      </c>
+      <c r="C8">
         <v>8</v>
+      </c>
+      <c r="D8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>2013011009</v>
+      </c>
+      <c r="B9">
+        <v>3.91</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2013011010</v>
+      </c>
+      <c r="B10">
+        <v>3.9</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2013011011</v>
+      </c>
+      <c r="B11">
+        <v>3.89</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2013011012</v>
+      </c>
+      <c r="B12">
+        <v>3.88</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2013011013</v>
+      </c>
+      <c r="B13">
+        <v>3.87</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2013011014</v>
+      </c>
+      <c r="B14">
+        <v>3.86</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>2013011015</v>
+      </c>
+      <c r="B15">
+        <v>3.85</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>2013011016</v>
+      </c>
+      <c r="B16">
+        <v>3.84</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2013011017</v>
+      </c>
+      <c r="B17">
+        <v>3.83</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>2013011018</v>
+      </c>
+      <c r="B18">
+        <v>3.82</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>2013011019</v>
+      </c>
+      <c r="B19">
+        <v>3.81</v>
+      </c>
+      <c r="C19">
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>2013011020</v>
+      </c>
+      <c r="B20">
+        <v>3.8</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>2013011021</v>
+      </c>
+      <c r="B21">
+        <v>3.79</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>2013011022</v>
+      </c>
+      <c r="B22">
+        <v>3.78</v>
+      </c>
+      <c r="C22">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>2013011023</v>
+      </c>
+      <c r="B23">
+        <v>3.77</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>2013011024</v>
+      </c>
+      <c r="B24">
+        <v>3.76</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>2013011025</v>
+      </c>
+      <c r="B25">
+        <v>3.7499999999999898</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>2013011026</v>
+      </c>
+      <c r="B26">
+        <v>3.73999999999999</v>
+      </c>
+      <c r="C26">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>2013011027</v>
+      </c>
+      <c r="B27">
+        <v>3.7299999999999902</v>
+      </c>
+      <c r="C27">
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>2013011028</v>
+      </c>
+      <c r="B28">
+        <v>3.71999999999999</v>
+      </c>
+      <c r="C28">
+        <v>28</v>
+      </c>
+      <c r="D28">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>2013011029</v>
+      </c>
+      <c r="B29">
+        <v>3.7099999999999902</v>
+      </c>
+      <c r="C29">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>